<commit_message>
Changed URL to another HRM
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/Details.xlsx
+++ b/src/test/java/testdata/Details.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -24,19 +24,37 @@
     <t>password</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>harleen</t>
-  </si>
-  <si>
-    <t>test123</t>
-  </si>
-  <si>
-    <t>test</t>
+    <t>sentrifugo</t>
+  </si>
+  <si>
+    <t>EM06</t>
+  </si>
+  <si>
+    <t>EM01</t>
+  </si>
+  <si>
+    <t>EM02</t>
+  </si>
+  <si>
+    <t>EM03</t>
+  </si>
+  <si>
+    <t>EM04</t>
+  </si>
+  <si>
+    <t>EM05</t>
+  </si>
+  <si>
+    <t>EM07</t>
+  </si>
+  <si>
+    <t>EM08</t>
+  </si>
+  <si>
+    <t>AGCY8</t>
+  </si>
+  <si>
+    <t>US09</t>
   </si>
 </sst>
 </file>
@@ -375,13 +393,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -393,18 +414,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -412,11 +433,68 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Testing with Excel File
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/Details.xlsx
+++ b/src/test/java/testdata/Details.xlsx
@@ -90,8 +90,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,7 +399,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,90 +408,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>